<commit_message>
test for login and search
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="505">
   <si>
     <t>単体テスト</t>
     <rPh sb="0" eb="2">
@@ -4636,6 +4636,814 @@
   </si>
   <si>
     <t>NO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12ー1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>login.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メールアドレス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パスワード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボタン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログイン画面表示</t>
+    <rPh sb="4" eb="6">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>urlなどに直接打ち込んでlogin.phpに入る。</t>
+    <rPh sb="6" eb="8">
+      <t>チョクセツ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ハイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>login.phpに遷移したとき、メールアドレスのテキストボックスが表示されている。初期値は空欄で、最大100文字まで。</t>
+    <rPh sb="10" eb="12">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="42" eb="45">
+      <t>ショキチ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>クウラン</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>サイダイ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>モジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>login.phpに遷移したとき、ログインボタンが配置されている。</t>
+    <rPh sb="10" eb="12">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ハイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>login.phpに遷移したとき、パスワードのテキストボックスが表示されている。初期値は空欄で、最大10文字まで。</t>
+    <rPh sb="10" eb="12">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="40" eb="43">
+      <t>ショキチ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>クウラン</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>サイダイ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>モジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12ー2</t>
+  </si>
+  <si>
+    <t>12ー3</t>
+  </si>
+  <si>
+    <t>13ー1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウント登録</t>
+    <rPh sb="5" eb="7">
+      <t>トウロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウント一覧</t>
+    <rPh sb="5" eb="7">
+      <t>イチラン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13ー2</t>
+  </si>
+  <si>
+    <t>リスト一覧画面</t>
+    <rPh sb="3" eb="5">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>login.phpから「ログイン」ボタンを押して、遷移させる。</t>
+    <rPh sb="21" eb="22">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>センイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログインしたアカウントによって、表示させるかさせないか区別する。アカウント権限が「一般」のときは、表示させない。「管理者」のときは、表示させる。</t>
+    <rPh sb="16" eb="18">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>クベツ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ケンゲン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="57" eb="60">
+      <t>カンリシャ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>初期画面</t>
+    <rPh sb="0" eb="2">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>イチガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index.php</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>14ー1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.2)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.2)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名前（姓）</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>セイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名前（名）</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カナ（姓）</t>
+    <rPh sb="3" eb="4">
+      <t>セイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カナ（名）</t>
+    <rPh sb="3" eb="4">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メールアドレス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>性別</t>
+    <rPh sb="0" eb="2">
+      <t>セイベツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウント権限</t>
+    <rPh sb="5" eb="7">
+      <t>ケンゲン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボタン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.2)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index.phpからlist.phpに遷移させる。</t>
+    <rPh sb="20" eb="22">
+      <t>センイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。名前（姓）のみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が1つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="144" eb="148">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="161" eb="163">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="171" eb="173">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。名前（名）のみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が2つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="144" eb="148">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="161" eb="163">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="171" eb="173">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>14ー2</t>
+  </si>
+  <si>
+    <t>14ー3</t>
+  </si>
+  <si>
+    <t>14ー4</t>
+  </si>
+  <si>
+    <t>14ー5</t>
+  </si>
+  <si>
+    <t>14ー6</t>
+  </si>
+  <si>
+    <t>14ー7</t>
+  </si>
+  <si>
+    <t>14ー8</t>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。カナ（姓）のみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が3つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="144" eb="148">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="161" eb="163">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="171" eb="173">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。カナ（名）のみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が4つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="144" eb="148">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="161" eb="163">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="171" eb="173">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。メールアドレスのみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が5つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="146" eb="150">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="151" eb="153">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="163" eb="165">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="173" eb="175">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>検索フォームの右下に「検索」ボタンが表示されている。</t>
+    <rPh sb="0" eb="2">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ミギシタ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。性別のみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が6つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。初期値は「男」。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>セイベツ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="141" eb="145">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="146" eb="148">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="158" eb="160">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="168" eb="170">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="174" eb="177">
+      <t>ショキチ</t>
+    </rPh>
+    <rPh sb="179" eb="180">
+      <t>オトコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>list.php (ver.1)のときは、最初に遷移した段階でアカウントが一覧として表示されたが、ver.2では検索機能を追加している。アカウント権限のみで検索をかけたとき、それを表示させる。また1文字以上で検索をかけたとき、その文字が7つでも適合していれば、そのアカウントも表示させる。また複数項目で検索をかけたとき、それに該当するアカウントも表示させる。初期値は「一般」。</t>
+    <rPh sb="21" eb="23">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>センイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダンカイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ケンゲン</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="99" eb="101">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>テキゴウ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="146" eb="150">
+      <t>フクスウコウモク</t>
+    </rPh>
+    <rPh sb="151" eb="153">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="163" eb="165">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="173" eb="175">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="179" eb="182">
+      <t>ショキチ</t>
+    </rPh>
+    <rPh sb="184" eb="186">
+      <t>イッパン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>柴田</t>
+    <rPh sb="0" eb="2">
+      <t>シバタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OK</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4849,7 +5657,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4960,6 +5768,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5241,10 +6052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I152" sqref="I152"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I195" sqref="I195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -5302,7 +6113,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
@@ -5335,7 +6146,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -5368,7 +6179,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -5401,7 +6212,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -5434,7 +6245,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -5467,7 +6278,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -5500,7 +6311,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -5533,7 +6344,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -5566,7 +6377,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -5599,7 +6410,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -5632,7 +6443,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -5665,7 +6476,7 @@
         <v>45393</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -6616,7 +7427,7 @@
       <c r="J44" s="5"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>155</v>
       </c>
@@ -6649,7 +7460,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>156</v>
       </c>
@@ -6682,7 +7493,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>157</v>
       </c>
@@ -6715,7 +7526,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>158</v>
       </c>
@@ -6748,7 +7559,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>159</v>
       </c>
@@ -6814,7 +7625,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>161</v>
       </c>
@@ -6847,7 +7658,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>162</v>
       </c>
@@ -6880,7 +7691,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>163</v>
       </c>
@@ -6913,7 +7724,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>164</v>
       </c>
@@ -6946,7 +7757,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>165</v>
       </c>
@@ -6979,7 +7790,7 @@
         <v>45394</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>166</v>
       </c>
@@ -7591,7 +8402,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>208</v>
       </c>
@@ -7624,7 +8435,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>209</v>
       </c>
@@ -7657,7 +8468,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>210</v>
       </c>
@@ -7690,7 +8501,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>211</v>
       </c>
@@ -7756,7 +8567,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>213</v>
       </c>
@@ -7789,7 +8600,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>214</v>
       </c>
@@ -7822,7 +8633,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>215</v>
       </c>
@@ -7855,7 +8666,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>216</v>
       </c>
@@ -7888,7 +8699,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>217</v>
       </c>
@@ -7921,7 +8732,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>218</v>
       </c>
@@ -8085,7 +8896,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
         <v>249</v>
       </c>
@@ -8118,7 +8929,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
         <v>250</v>
       </c>
@@ -8151,7 +8962,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
         <v>251</v>
       </c>
@@ -8184,7 +8995,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
         <v>252</v>
       </c>
@@ -8217,7 +9028,7 @@
         <v>45403</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
         <v>253</v>
       </c>
@@ -10039,6 +10850,435 @@
       </c>
       <c r="K157" s="32">
         <v>45425</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A159" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F159" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="G159" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J159" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K159" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A160" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F160" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="G160" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J160" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K160" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A161" s="34" t="s">
+        <v>464</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F161" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="G161" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J161" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K161" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A163" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="G163" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H163" s="1"/>
+      <c r="I163" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J163" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K163" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A164" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="F164" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="G164" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H164" s="1"/>
+      <c r="I164" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J164" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K164" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F166" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G166" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="H166" s="1"/>
+      <c r="I166" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K166" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F167" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G167" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J167" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K167" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F168" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G168" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K168" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F169" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G169" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="J169" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K169" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F170" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G170" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="H170" s="1"/>
+      <c r="I170" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K170" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F171" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G171" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K171" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F172" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G172" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="H172" s="1"/>
+      <c r="I172" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K172" s="32">
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F173" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="G173" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="H173" s="1"/>
+      <c r="I173" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J173" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K173" s="32">
+        <v>45436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>